<commit_message>
get data from config
</commit_message>
<xml_diff>
--- a/users.xlsx
+++ b/users.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MyProject\AcademyLearning\FinalProject\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{851BD053-F177-4102-9766-9E9E2E691679}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CD9F190-3BDD-48B2-A324-71BC59D854F0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" xr2:uid="{FBDC5C77-C85C-4E20-98D2-48155EC339ED}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" xr2:uid="{F37E7966-8F41-4060-AC40-F959AD162744}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -48,43 +48,43 @@
     <t>status</t>
   </si>
   <si>
-    <t>George L. Perry</t>
-  </si>
-  <si>
-    <t>GeorgeLPerry@rhyta.com            This is a real email address. Click here to activate it!</t>
+    <t>John T. Hawkins</t>
+  </si>
+  <si>
+    <t>JohnTHawkins@jourrapide.com            This is a real email address. Click here to activate it!</t>
   </si>
   <si>
     <t xml:space="preserve">
-                                        1466 Ferrell StreetDuluth, MN 55802                                        </t>
-  </si>
-  <si>
-    <t>218-406-6514</t>
-  </si>
-  <si>
-    <t>Arlene E. Porter</t>
-  </si>
-  <si>
-    <t>ArleneEPorter@teleworm.us            This is a real email address. Click here to activate it!</t>
+                                        3538 Filbert StreetChester, PA 19013                                        </t>
+  </si>
+  <si>
+    <t>610-876-7584</t>
+  </si>
+  <si>
+    <t>Beverly J. Chambers</t>
+  </si>
+  <si>
+    <t>BeverlyJChambers@teleworm.us            This is a real email address. Click here to activate it!</t>
   </si>
   <si>
     <t xml:space="preserve">
-                                        3347 Parrish AvenueFredericksburg, TX 78624                                        </t>
-  </si>
-  <si>
-    <t>830-997-5768</t>
-  </si>
-  <si>
-    <t>Douglas M. Saenz</t>
-  </si>
-  <si>
-    <t>DouglasMSaenz@jourrapide.com            This is a real email address. Click here to activate it!</t>
+                                        4055 Pallet StreetWest Nyack, NY 10994                                        </t>
+  </si>
+  <si>
+    <t>914-346-4627</t>
+  </si>
+  <si>
+    <t>Gordon P. Fields</t>
+  </si>
+  <si>
+    <t>GordonPFields@teleworm.us            This is a real email address. Click here to activate it!</t>
   </si>
   <si>
     <t xml:space="preserve">
-                                        2787 Cherry Ridge DriveRochester, NY 14620                                        </t>
-  </si>
-  <si>
-    <t>585-784-1072</t>
+                                        4402 Modoc AlleyDixie, ID 83525                                        </t>
+  </si>
+  <si>
+    <t>208-842-0461</t>
   </si>
   <si>
     <t>ok</t>
@@ -441,7 +441,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{90D28A0E-3BA5-4E7C-8C34-EAFB1D7B62FC}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3E46EB43-8B64-4316-91FB-F30DA84B55CD}">
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
@@ -482,7 +482,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="114" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:5" ht="99.75" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -499,7 +499,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="114" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:5" ht="85.5" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>13</v>
       </c>

</xml_diff>